<commit_message>
chore - Commiting uncommited changes.
</commit_message>
<xml_diff>
--- a/data/processed/AUC vs n_estimators vs depth.xlsx
+++ b/data/processed/AUC vs n_estimators vs depth.xlsx
@@ -420,34 +420,34 @@
         <v>75</v>
       </c>
       <c r="B2">
-        <v>0.9985808968380991</v>
+        <v>0.9987358105160696</v>
       </c>
       <c r="C2">
-        <v>0.9986571277700793</v>
+        <v>0.9988174428688066</v>
       </c>
       <c r="D2">
-        <v>0.9986298070793678</v>
+        <v>0.9987085027441884</v>
       </c>
       <c r="E2">
-        <v>0.9986907995762498</v>
+        <v>0.9987364733613232</v>
       </c>
       <c r="F2">
-        <v>0.9987695151656346</v>
+        <v>0.9987417553632414</v>
       </c>
       <c r="G2">
-        <v>0.9987032326970086</v>
+        <v>0.9987695953138001</v>
       </c>
       <c r="H2">
-        <v>0.9986829061709912</v>
+        <v>0.9987695953138001</v>
       </c>
       <c r="I2">
-        <v>0.9987285118269101</v>
+        <v>0.9987695953138001</v>
       </c>
       <c r="J2">
-        <v>0.9987285118269101</v>
+        <v>0.9987695953138001</v>
       </c>
       <c r="K2">
-        <v>0.9987285118269101</v>
+        <v>0.9987695953138001</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -455,34 +455,34 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>0.9987511476098959</v>
+        <v>0.9988579196205862</v>
       </c>
       <c r="C3">
-        <v>0.9987309845938489</v>
+        <v>0.9988249643274463</v>
       </c>
       <c r="D3">
-        <v>0.9987365574944016</v>
+        <v>0.9987847937712242</v>
       </c>
       <c r="E3">
-        <v>0.9987164369626669</v>
+        <v>0.9987646892434139</v>
       </c>
       <c r="F3">
-        <v>0.9988153741206076</v>
+        <v>0.9987518825692165</v>
       </c>
       <c r="G3">
-        <v>0.9987618590555056</v>
+        <v>0.998838015431053</v>
       </c>
       <c r="H3">
-        <v>0.9987466574487149</v>
+        <v>0.998838015431053</v>
       </c>
       <c r="I3">
-        <v>0.9987694398379281</v>
+        <v>0.998838015431053</v>
       </c>
       <c r="J3">
-        <v>0.9987694398379281</v>
+        <v>0.998838015431053</v>
       </c>
       <c r="K3">
-        <v>0.9987694398379281</v>
+        <v>0.998838015431053</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -490,34 +490,34 @@
         <v>125</v>
       </c>
       <c r="B4">
-        <v>0.9988529101352854</v>
+        <v>0.9988478685778637</v>
       </c>
       <c r="C4">
-        <v>0.9987538639706978</v>
+        <v>0.9988503011743106</v>
       </c>
       <c r="D4">
-        <v>0.9987517607080122</v>
+        <v>0.9988332303863249</v>
       </c>
       <c r="E4">
-        <v>0.9987619608636006</v>
+        <v>0.9987696097751773</v>
       </c>
       <c r="F4">
-        <v>0.9988254195715974</v>
+        <v>0.9987723197087007</v>
       </c>
       <c r="G4">
-        <v>0.9987693564761232</v>
+        <v>0.9988634259988041</v>
       </c>
       <c r="H4">
-        <v>0.9987110972437859</v>
+        <v>0.9988634259988041</v>
       </c>
       <c r="I4">
-        <v>0.9986576431092866</v>
+        <v>0.9988634259988041</v>
       </c>
       <c r="J4">
-        <v>0.9986576431092866</v>
+        <v>0.9988634259988041</v>
       </c>
       <c r="K4">
-        <v>0.9986576431092866</v>
+        <v>0.9988634259988041</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -525,34 +525,34 @@
         <v>150</v>
       </c>
       <c r="B5">
-        <v>0.9988833959393985</v>
+        <v>0.9988860112633791</v>
       </c>
       <c r="C5">
-        <v>0.9987766736115727</v>
+        <v>0.9989037873809309</v>
       </c>
       <c r="D5">
-        <v>0.9987569361456494</v>
+        <v>0.9988076274501216</v>
       </c>
       <c r="E5">
-        <v>0.9987465091713951</v>
+        <v>0.9987670377067823</v>
       </c>
       <c r="F5">
-        <v>0.9987823146412798</v>
+        <v>0.998800119617313</v>
       </c>
       <c r="G5">
-        <v>0.9987213799256333</v>
+        <v>0.9989370511834489</v>
       </c>
       <c r="H5">
-        <v>0.9986553571833398</v>
+        <v>0.9989370511834489</v>
       </c>
       <c r="I5">
-        <v>0.9985868040214176</v>
+        <v>0.9989370511834489</v>
       </c>
       <c r="J5">
-        <v>0.9985868040214176</v>
+        <v>0.9989370511834489</v>
       </c>
       <c r="K5">
-        <v>0.9985868040214176</v>
+        <v>0.9989370511834489</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -560,34 +560,34 @@
         <v>175</v>
       </c>
       <c r="B6">
-        <v>0.9988861483572341</v>
+        <v>0.9988477603424902</v>
       </c>
       <c r="C6">
-        <v>0.9987462743829036</v>
+        <v>0.9988300515828193</v>
       </c>
       <c r="D6">
-        <v>0.9987773203886293</v>
+        <v>0.9988661367678736</v>
       </c>
       <c r="E6">
-        <v>0.9987566500032011</v>
+        <v>0.9987875549944318</v>
       </c>
       <c r="F6">
-        <v>0.9987646010611499</v>
+        <v>0.9987950508082296</v>
       </c>
       <c r="G6">
-        <v>0.998695981376893</v>
+        <v>0.9989624273009863</v>
       </c>
       <c r="H6">
-        <v>0.9986402613695565</v>
+        <v>0.9989624273009863</v>
       </c>
       <c r="I6">
-        <v>0.9985614976398545</v>
+        <v>0.9989624273009863</v>
       </c>
       <c r="J6">
-        <v>0.9985614976398545</v>
+        <v>0.9989624273009863</v>
       </c>
       <c r="K6">
-        <v>0.9985614976398545</v>
+        <v>0.9989624273009863</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -595,34 +595,34 @@
         <v>200</v>
       </c>
       <c r="B7">
-        <v>0.9989268046229082</v>
+        <v>0.9988402236512</v>
       </c>
       <c r="C7">
-        <v>0.9987259670744496</v>
+        <v>0.9987817584245799</v>
       </c>
       <c r="D7">
-        <v>0.9987492800355205</v>
+        <v>0.9988229052201654</v>
       </c>
       <c r="E7">
-        <v>0.9987236121838026</v>
+        <v>0.998833216760494</v>
       </c>
       <c r="F7">
-        <v>0.9987216284042282</v>
+        <v>0.9987950083239172</v>
       </c>
       <c r="G7">
-        <v>0.9987188880054036</v>
+        <v>0.9989523610256134</v>
       </c>
       <c r="H7">
-        <v>0.9986224323555011</v>
+        <v>0.9989523610256134</v>
       </c>
       <c r="I7">
-        <v>0.9986019799833665</v>
+        <v>0.9989523610256134</v>
       </c>
       <c r="J7">
-        <v>0.9986019799833665</v>
+        <v>0.9989523610256134</v>
       </c>
       <c r="K7">
-        <v>0.9986019799833665</v>
+        <v>0.9989523610256134</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -630,34 +630,34 @@
         <v>225</v>
       </c>
       <c r="B8">
-        <v>0.9989318670047128</v>
+        <v>0.9988402220443803</v>
       </c>
       <c r="C8">
-        <v>0.9987260864932882</v>
+        <v>0.9987818978965279</v>
       </c>
       <c r="D8">
-        <v>0.9987238165712655</v>
+        <v>0.9988382190472425</v>
       </c>
       <c r="E8">
-        <v>0.9986855520245458</v>
+        <v>0.9988103967074273</v>
       </c>
       <c r="F8">
-        <v>0.998698941395831</v>
+        <v>0.9987621019423683</v>
       </c>
       <c r="G8">
-        <v>0.9987214224099453</v>
+        <v>0.9989524836580912</v>
       </c>
       <c r="H8">
-        <v>0.9986172665587821</v>
+        <v>0.9989524836580912</v>
       </c>
       <c r="I8">
-        <v>0.9986171607657743</v>
+        <v>0.9989524836580912</v>
       </c>
       <c r="J8">
-        <v>0.9986171607657743</v>
+        <v>0.9989524836580912</v>
       </c>
       <c r="K8">
-        <v>0.9986171607657743</v>
+        <v>0.9989524836580912</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -665,34 +665,34 @@
         <v>250</v>
       </c>
       <c r="B9">
-        <v>0.9989090164863453</v>
+        <v>0.9988402284716589</v>
       </c>
       <c r="C9">
-        <v>0.9987185001191335</v>
+        <v>0.9987514850420283</v>
       </c>
       <c r="D9">
-        <v>0.9987340583756202</v>
+        <v>0.9988230382648347</v>
       </c>
       <c r="E9">
-        <v>0.998680575382639</v>
+        <v>0.9988205599704362</v>
       </c>
       <c r="F9">
-        <v>0.9987598079823232</v>
+        <v>0.9987367458779406</v>
       </c>
       <c r="G9">
-        <v>0.9987010213274949</v>
+        <v>0.9989143433506689</v>
       </c>
       <c r="H9">
-        <v>0.9985867158391539</v>
+        <v>0.9989143433506689</v>
       </c>
       <c r="I9">
-        <v>0.9986120374533677</v>
+        <v>0.9989143433506689</v>
       </c>
       <c r="J9">
-        <v>0.9986120374533677</v>
+        <v>0.9989143433506689</v>
       </c>
       <c r="K9">
-        <v>0.9986120374533677</v>
+        <v>0.9989143433506689</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -700,34 +700,34 @@
         <v>275</v>
       </c>
       <c r="B10">
-        <v>0.9989039356582508</v>
+        <v>0.9988402148458281</v>
       </c>
       <c r="C10">
-        <v>0.9987263285446046</v>
+        <v>0.9987668838377299</v>
       </c>
       <c r="D10">
-        <v>0.998759454546267</v>
+        <v>0.9988612058239186</v>
       </c>
       <c r="E10">
-        <v>0.9986348198425808</v>
+        <v>0.9988053687758368</v>
       </c>
       <c r="F10">
-        <v>0.9987597807306617</v>
+        <v>0.9987393844686702</v>
       </c>
       <c r="G10">
-        <v>0.9986883509116063</v>
+        <v>0.9988458479057096</v>
       </c>
       <c r="H10">
-        <v>0.9986197192083383</v>
+        <v>0.9988458479057096</v>
       </c>
       <c r="I10">
-        <v>0.998599348591189</v>
+        <v>0.9988458479057096</v>
       </c>
       <c r="J10">
-        <v>0.998599348591189</v>
+        <v>0.9988458479057096</v>
       </c>
       <c r="K10">
-        <v>0.998599348591189</v>
+        <v>0.9988458479057096</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -735,34 +735,34 @@
         <v>300</v>
       </c>
       <c r="B11">
-        <v>0.9989013227123632</v>
+        <v>0.9988224315297242</v>
       </c>
       <c r="C11">
-        <v>0.9987467312338746</v>
+        <v>0.9987440044608811</v>
       </c>
       <c r="D11">
-        <v>0.9987646002898766</v>
+        <v>0.9987572102690864</v>
       </c>
       <c r="E11">
-        <v>0.9986754536770521</v>
+        <v>0.9986301934873639</v>
       </c>
       <c r="F11">
-        <v>0.9987546999025672</v>
+        <v>0.9987469876822951</v>
       </c>
       <c r="G11">
-        <v>0.9986984492591</v>
+        <v>0.9988406684831597</v>
       </c>
       <c r="H11">
-        <v>0.9986044686899564</v>
+        <v>0.9988406684831597</v>
       </c>
       <c r="I11">
-        <v>0.9985790292637239</v>
+        <v>0.9988406684831597</v>
       </c>
       <c r="J11">
-        <v>0.9985790292637239</v>
+        <v>0.9988406684831597</v>
       </c>
       <c r="K11">
-        <v>0.9985790292637239</v>
+        <v>0.9988406684831597</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -770,34 +770,34 @@
         <v>325</v>
       </c>
       <c r="B12">
-        <v>0.9989141021348988</v>
+        <v>0.9988302255049815</v>
       </c>
       <c r="C12">
-        <v>0.9987086350175842</v>
+        <v>0.9987592894294769</v>
       </c>
       <c r="D12">
-        <v>0.9987417377524977</v>
+        <v>0.9987293558571505</v>
       </c>
       <c r="E12">
-        <v>0.9986779015061495</v>
+        <v>0.9986404080400566</v>
       </c>
       <c r="F12">
-        <v>0.9987495645711493</v>
+        <v>0.9987494932283554</v>
       </c>
       <c r="G12">
-        <v>0.9986959132477388</v>
+        <v>0.9988051018509519</v>
       </c>
       <c r="H12">
-        <v>0.9986298568265051</v>
+        <v>0.9988051018509519</v>
       </c>
       <c r="I12">
-        <v>0.9985917285380939</v>
+        <v>0.9988051018509519</v>
       </c>
       <c r="J12">
-        <v>0.9985917285380939</v>
+        <v>0.9988051018509519</v>
       </c>
       <c r="K12">
-        <v>0.9985917285380939</v>
+        <v>0.9988051018509519</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -805,34 +805,34 @@
         <v>350</v>
       </c>
       <c r="B13">
-        <v>0.9988760179376197</v>
+        <v>0.9987921757579162</v>
       </c>
       <c r="C13">
-        <v>0.9986757134033848</v>
+        <v>0.9987108512075569</v>
       </c>
       <c r="D13">
-        <v>0.9987112567688439</v>
+        <v>0.9987394950821369</v>
       </c>
       <c r="E13">
-        <v>0.9986549964844584</v>
+        <v>0.9986479992346704</v>
       </c>
       <c r="F13">
-        <v>0.9987672765444593</v>
+        <v>0.9987596685103753</v>
       </c>
       <c r="G13">
-        <v>0.9986984492591</v>
+        <v>0.9987999937711957</v>
       </c>
       <c r="H13">
-        <v>0.9986374159489981</v>
+        <v>0.9987999937711957</v>
       </c>
       <c r="I13">
-        <v>0.9986170333128376</v>
+        <v>0.9987999937711957</v>
       </c>
       <c r="J13">
-        <v>0.9986170333128376</v>
+        <v>0.9987999937711957</v>
       </c>
       <c r="K13">
-        <v>0.9986170333128376</v>
+        <v>0.9987999937711957</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -840,34 +840,34 @@
         <v>375</v>
       </c>
       <c r="B14">
-        <v>0.9988454992901122</v>
+        <v>0.9987640945273146</v>
       </c>
       <c r="C14">
-        <v>0.9986733529210051</v>
+        <v>0.9986675908013671</v>
       </c>
       <c r="D14">
-        <v>0.9986580222544579</v>
+        <v>0.9987648663792152</v>
       </c>
       <c r="E14">
-        <v>0.998665147728456</v>
+        <v>0.998647970376189</v>
       </c>
       <c r="F14">
-        <v>0.9987495357126678</v>
+        <v>0.9987647373194586</v>
       </c>
       <c r="G14">
-        <v>0.998700970037811</v>
+        <v>0.9988203082782018</v>
       </c>
       <c r="H14">
-        <v>0.9986475808188263</v>
+        <v>0.9988203082782018</v>
       </c>
       <c r="I14">
-        <v>0.9986094421182239</v>
+        <v>0.9988203082782018</v>
       </c>
       <c r="J14">
-        <v>0.9986094421182239</v>
+        <v>0.9988203082782018</v>
       </c>
       <c r="K14">
-        <v>0.9986094421182239</v>
+        <v>0.9988203082782018</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -875,34 +875,34 @@
         <v>400</v>
       </c>
       <c r="B15">
-        <v>0.9988277945153543</v>
+        <v>0.9987666545766982</v>
       </c>
       <c r="C15">
-        <v>0.9987112615893026</v>
+        <v>0.9986575197055354</v>
       </c>
       <c r="D15">
-        <v>0.9986580631319502</v>
+        <v>0.9987826601075105</v>
       </c>
       <c r="E15">
-        <v>0.9986422427067649</v>
+        <v>0.9986607361728937</v>
       </c>
       <c r="F15">
-        <v>0.9987673174219518</v>
+        <v>0.9987799742120096</v>
       </c>
       <c r="G15">
-        <v>0.9987085732514359</v>
+        <v>0.9988305140255228</v>
       </c>
       <c r="H15">
-        <v>0.9986551840324512</v>
+        <v>0.9988305140255228</v>
       </c>
       <c r="I15">
-        <v>0.9986246485454737</v>
+        <v>0.9988305140255228</v>
       </c>
       <c r="J15">
-        <v>0.9986246485454737</v>
+        <v>0.9988305140255228</v>
       </c>
       <c r="K15">
-        <v>0.9986246485454737</v>
+        <v>0.9988305140255228</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -910,34 +910,34 @@
         <v>425</v>
       </c>
       <c r="B16">
-        <v>0.9988354265874607</v>
+        <v>0.99877171297359</v>
       </c>
       <c r="C16">
-        <v>0.9986783159370809</v>
+        <v>0.9985964471247601</v>
       </c>
       <c r="D16">
-        <v>0.9986555134947579</v>
+        <v>0.9987674007837567</v>
       </c>
       <c r="E16">
-        <v>0.9986345729708054</v>
+        <v>0.9986327214646268</v>
       </c>
       <c r="F16">
-        <v>0.9987596580981837</v>
+        <v>0.9987774518264791</v>
       </c>
       <c r="G16">
-        <v>0.9987110940301467</v>
+        <v>0.9988355692087753</v>
       </c>
       <c r="H16">
-        <v>0.9986678833068213</v>
+        <v>0.9988355692087753</v>
       </c>
       <c r="I16">
-        <v>0.9986297446062189</v>
+        <v>0.9988355692087753</v>
       </c>
       <c r="J16">
-        <v>0.9986297446062189</v>
+        <v>0.9988355692087753</v>
       </c>
       <c r="K16">
-        <v>0.9986297446062189</v>
+        <v>0.9988355692087753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Adding two notebooks ("Artigo - ..." preffix).
</commit_message>
<xml_diff>
--- a/data/processed/AUC vs n_estimators vs depth.xlsx
+++ b/data/processed/AUC vs n_estimators vs depth.xlsx
@@ -420,34 +420,34 @@
         <v>75</v>
       </c>
       <c r="B2">
-        <v>0.9987358105160696</v>
+        <v>0.9952198296780035</v>
       </c>
       <c r="C2">
-        <v>0.9988174428688066</v>
+        <v>0.9966355433679656</v>
       </c>
       <c r="D2">
-        <v>0.9987085027441884</v>
+        <v>0.9975102775629839</v>
       </c>
       <c r="E2">
-        <v>0.9987364733613232</v>
+        <v>0.9976895517409459</v>
       </c>
       <c r="F2">
-        <v>0.9987417553632414</v>
+        <v>0.9977780323774856</v>
       </c>
       <c r="G2">
-        <v>0.9987695953138001</v>
+        <v>0.9979106895813292</v>
       </c>
       <c r="H2">
-        <v>0.9987695953138001</v>
+        <v>0.9979310951673991</v>
       </c>
       <c r="I2">
-        <v>0.9987695953138001</v>
+        <v>0.9979310951673991</v>
       </c>
       <c r="J2">
-        <v>0.9987695953138001</v>
+        <v>0.9979310951673991</v>
       </c>
       <c r="K2">
-        <v>0.9987695953138001</v>
+        <v>0.9979310951673991</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -455,34 +455,34 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>0.9988579196205862</v>
+        <v>0.9965419272583844</v>
       </c>
       <c r="C3">
-        <v>0.9988249643274463</v>
+        <v>0.9975325122933653</v>
       </c>
       <c r="D3">
-        <v>0.9987847937712242</v>
+        <v>0.9979647285346575</v>
       </c>
       <c r="E3">
-        <v>0.9987646892434139</v>
+        <v>0.9980989918439891</v>
       </c>
       <c r="F3">
-        <v>0.9987518825692165</v>
+        <v>0.9981973039624215</v>
       </c>
       <c r="G3">
-        <v>0.998838015431053</v>
+        <v>0.9983213873158107</v>
       </c>
       <c r="H3">
-        <v>0.998838015431053</v>
+        <v>0.9983213566321274</v>
       </c>
       <c r="I3">
-        <v>0.998838015431053</v>
+        <v>0.9983213566321274</v>
       </c>
       <c r="J3">
-        <v>0.998838015431053</v>
+        <v>0.9983213566321274</v>
       </c>
       <c r="K3">
-        <v>0.998838015431053</v>
+        <v>0.9983213566321274</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -490,34 +490,34 @@
         <v>125</v>
       </c>
       <c r="B4">
-        <v>0.9988478685778637</v>
+        <v>0.9972234772335373</v>
       </c>
       <c r="C4">
-        <v>0.9988503011743106</v>
+        <v>0.9979103149979037</v>
       </c>
       <c r="D4">
-        <v>0.9988332303863249</v>
+        <v>0.9982356133879371</v>
       </c>
       <c r="E4">
-        <v>0.9987696097751773</v>
+        <v>0.9982712346362428</v>
       </c>
       <c r="F4">
-        <v>0.9987723197087007</v>
+        <v>0.9983849319969604</v>
       </c>
       <c r="G4">
-        <v>0.9988634259988041</v>
+        <v>0.9984969085500521</v>
       </c>
       <c r="H4">
-        <v>0.9988634259988041</v>
+        <v>0.9984868851401382</v>
       </c>
       <c r="I4">
-        <v>0.9988634259988041</v>
+        <v>0.998484386493572</v>
       </c>
       <c r="J4">
-        <v>0.9988634259988041</v>
+        <v>0.998484386493572</v>
       </c>
       <c r="K4">
-        <v>0.9988634259988041</v>
+        <v>0.998484386493572</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -525,34 +525,34 @@
         <v>150</v>
       </c>
       <c r="B5">
-        <v>0.9988860112633791</v>
+        <v>0.9975920874952038</v>
       </c>
       <c r="C5">
-        <v>0.9989037873809309</v>
+        <v>0.9981125075585437</v>
       </c>
       <c r="D5">
-        <v>0.9988076274501216</v>
+        <v>0.9983961471241953</v>
       </c>
       <c r="E5">
-        <v>0.9987670377067823</v>
+        <v>0.9984152138435354</v>
       </c>
       <c r="F5">
-        <v>0.998800119617313</v>
+        <v>0.9985027035638299</v>
       </c>
       <c r="G5">
-        <v>0.9989370511834489</v>
+        <v>0.9986125620747819</v>
       </c>
       <c r="H5">
-        <v>0.9989370511834489</v>
+        <v>0.9986125338711451</v>
       </c>
       <c r="I5">
-        <v>0.9989370511834489</v>
+        <v>0.9986100352245787</v>
       </c>
       <c r="J5">
-        <v>0.9989370511834489</v>
+        <v>0.9986100352245787</v>
       </c>
       <c r="K5">
-        <v>0.9989370511834489</v>
+        <v>0.9986100352245787</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -560,34 +560,34 @@
         <v>175</v>
       </c>
       <c r="B6">
-        <v>0.9988477603424902</v>
+        <v>0.9978025686045369</v>
       </c>
       <c r="C6">
-        <v>0.9988300515828193</v>
+        <v>0.9982806191724727</v>
       </c>
       <c r="D6">
-        <v>0.9988661367678736</v>
+        <v>0.9984860350354063</v>
       </c>
       <c r="E6">
-        <v>0.9987875549944318</v>
+        <v>0.9984992837316511</v>
       </c>
       <c r="F6">
-        <v>0.9987950508082296</v>
+        <v>0.998588354164516</v>
       </c>
       <c r="G6">
-        <v>0.9989624273009863</v>
+        <v>0.9987206774301362</v>
       </c>
       <c r="H6">
-        <v>0.9989624273009863</v>
+        <v>0.9987298646924673</v>
       </c>
       <c r="I6">
-        <v>0.9989624273009863</v>
+        <v>0.9987157069766146</v>
       </c>
       <c r="J6">
-        <v>0.9989624273009863</v>
+        <v>0.9987157069766146</v>
       </c>
       <c r="K6">
-        <v>0.9989624273009863</v>
+        <v>0.9987157069766146</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -595,34 +595,34 @@
         <v>200</v>
       </c>
       <c r="B7">
-        <v>0.9988402236512</v>
+        <v>0.9979747115887083</v>
       </c>
       <c r="C7">
-        <v>0.9987817584245799</v>
+        <v>0.9983937477759239</v>
       </c>
       <c r="D7">
-        <v>0.9988229052201654</v>
+        <v>0.9985958660454013</v>
       </c>
       <c r="E7">
-        <v>0.998833216760494</v>
+        <v>0.9985924814298789</v>
       </c>
       <c r="F7">
-        <v>0.9987950083239172</v>
+        <v>0.9986615294300367</v>
       </c>
       <c r="G7">
-        <v>0.9989523610256134</v>
+        <v>0.9987630949419906</v>
       </c>
       <c r="H7">
-        <v>0.9989523610256134</v>
+        <v>0.9987547648111891</v>
       </c>
       <c r="I7">
-        <v>0.9989523610256134</v>
+        <v>0.9987564216198443</v>
       </c>
       <c r="J7">
-        <v>0.9989523610256134</v>
+        <v>0.9987564216198443</v>
       </c>
       <c r="K7">
-        <v>0.9989523610256134</v>
+        <v>0.9987564216198443</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -630,34 +630,34 @@
         <v>225</v>
       </c>
       <c r="B8">
-        <v>0.9988402220443803</v>
+        <v>0.9981153189389385</v>
       </c>
       <c r="C8">
-        <v>0.9987818978965279</v>
+        <v>0.9984952377980262</v>
       </c>
       <c r="D8">
-        <v>0.9988382190472425</v>
+        <v>0.9986407955960719</v>
       </c>
       <c r="E8">
-        <v>0.9988103967074273</v>
+        <v>0.9986349315405632</v>
       </c>
       <c r="F8">
-        <v>0.9987621019423683</v>
+        <v>0.9987081490633157</v>
       </c>
       <c r="G8">
-        <v>0.9989524836580912</v>
+        <v>0.9987822032296607</v>
       </c>
       <c r="H8">
-        <v>0.9989524836580912</v>
+        <v>0.9987872241934571</v>
       </c>
       <c r="I8">
-        <v>0.9989524836580912</v>
+        <v>0.9988055130463003</v>
       </c>
       <c r="J8">
-        <v>0.9989524836580912</v>
+        <v>0.9988055130463003</v>
       </c>
       <c r="K8">
-        <v>0.9989524836580912</v>
+        <v>0.9988055130463003</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -665,34 +665,34 @@
         <v>250</v>
       </c>
       <c r="B9">
-        <v>0.9988402284716589</v>
+        <v>0.9982213520888206</v>
       </c>
       <c r="C9">
-        <v>0.9987514850420283</v>
+        <v>0.9985593287644681</v>
       </c>
       <c r="D9">
-        <v>0.9988230382648347</v>
+        <v>0.9986465886671463</v>
       </c>
       <c r="E9">
-        <v>0.9988205599704362</v>
+        <v>0.9986398782958652</v>
       </c>
       <c r="F9">
-        <v>0.9987367458779406</v>
+        <v>0.99874890138947</v>
       </c>
       <c r="G9">
-        <v>0.9989143433506689</v>
+        <v>0.9987946491211662</v>
       </c>
       <c r="H9">
-        <v>0.9989143433506689</v>
+        <v>0.9988004799164996</v>
       </c>
       <c r="I9">
-        <v>0.9989143433506689</v>
+        <v>0.9988229357292233</v>
       </c>
       <c r="J9">
-        <v>0.9989143433506689</v>
+        <v>0.9988229357292233</v>
       </c>
       <c r="K9">
-        <v>0.9989143433506689</v>
+        <v>0.9988229357292233</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -700,34 +700,34 @@
         <v>275</v>
       </c>
       <c r="B10">
-        <v>0.9988402148458281</v>
+        <v>0.9982945772446044</v>
       </c>
       <c r="C10">
-        <v>0.9987668838377299</v>
+        <v>0.9986116979577886</v>
       </c>
       <c r="D10">
-        <v>0.9988612058239186</v>
+        <v>0.998646592511218</v>
       </c>
       <c r="E10">
-        <v>0.9988053687758368</v>
+        <v>0.9986764649710522</v>
       </c>
       <c r="F10">
-        <v>0.9987393844686702</v>
+        <v>0.9987588966233034</v>
       </c>
       <c r="G10">
-        <v>0.9988458479057096</v>
+        <v>0.998820449896229</v>
       </c>
       <c r="H10">
-        <v>0.9988458479057096</v>
+        <v>0.9988287601453265</v>
       </c>
       <c r="I10">
-        <v>0.9988458479057096</v>
+        <v>0.9988370755060749</v>
       </c>
       <c r="J10">
-        <v>0.9988458479057096</v>
+        <v>0.9988370755060749</v>
       </c>
       <c r="K10">
-        <v>0.9988458479057096</v>
+        <v>0.9988370755060749</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -735,34 +735,34 @@
         <v>300</v>
       </c>
       <c r="B11">
-        <v>0.9988224315297242</v>
+        <v>0.9983586221510772</v>
       </c>
       <c r="C11">
-        <v>0.9987440044608811</v>
+        <v>0.9986225414087633</v>
       </c>
       <c r="D11">
-        <v>0.9987572102690864</v>
+        <v>0.9986374327498438</v>
       </c>
       <c r="E11">
-        <v>0.9986301934873639</v>
+        <v>0.9987081074536516</v>
       </c>
       <c r="F11">
-        <v>0.9987469876822951</v>
+        <v>0.9987647031417397</v>
       </c>
       <c r="G11">
-        <v>0.9988406684831597</v>
+        <v>0.9988296103189487</v>
       </c>
       <c r="H11">
-        <v>0.9988406684831597</v>
+        <v>0.9988287332919373</v>
       </c>
       <c r="I11">
-        <v>0.9988406684831597</v>
+        <v>0.99884370530341</v>
       </c>
       <c r="J11">
-        <v>0.9988406684831597</v>
+        <v>0.99884370530341</v>
       </c>
       <c r="K11">
-        <v>0.9988406684831597</v>
+        <v>0.99884370530341</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -770,34 +770,34 @@
         <v>325</v>
       </c>
       <c r="B12">
-        <v>0.9988302255049815</v>
+        <v>0.9983852622013366</v>
       </c>
       <c r="C12">
-        <v>0.9987592894294769</v>
+        <v>0.9986366773690994</v>
       </c>
       <c r="D12">
-        <v>0.9987293558571505</v>
+        <v>0.9986332773221782</v>
       </c>
       <c r="E12">
-        <v>0.9986404080400566</v>
+        <v>0.9987239360593106</v>
       </c>
       <c r="F12">
-        <v>0.9987494932283554</v>
+        <v>0.9987505339074503</v>
       </c>
       <c r="G12">
-        <v>0.9988051018509519</v>
+        <v>0.9988237807774165</v>
       </c>
       <c r="H12">
-        <v>0.9988051018509519</v>
+        <v>0.9988253844855267</v>
       </c>
       <c r="I12">
-        <v>0.9988051018509519</v>
+        <v>0.9988228800659638</v>
       </c>
       <c r="J12">
-        <v>0.9988051018509519</v>
+        <v>0.9988228800659638</v>
       </c>
       <c r="K12">
-        <v>0.9988051018509519</v>
+        <v>0.9988228800659638</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -805,34 +805,34 @@
         <v>350</v>
       </c>
       <c r="B13">
-        <v>0.9987921757579162</v>
+        <v>0.9984176806215078</v>
       </c>
       <c r="C13">
-        <v>0.9987108512075569</v>
+        <v>0.9986632911997593</v>
       </c>
       <c r="D13">
-        <v>0.9987394950821369</v>
+        <v>0.9986490873550469</v>
       </c>
       <c r="E13">
-        <v>0.9986479992346704</v>
+        <v>0.9987339140017106</v>
       </c>
       <c r="F13">
-        <v>0.9987596685103753</v>
+        <v>0.9987588492819766</v>
       </c>
       <c r="G13">
-        <v>0.9987999937711957</v>
+        <v>0.9988362874438325</v>
       </c>
       <c r="H13">
-        <v>0.9987999937711957</v>
+        <v>0.998842014614568</v>
       </c>
       <c r="I13">
-        <v>0.9987999937711957</v>
+        <v>0.9988295373642557</v>
       </c>
       <c r="J13">
-        <v>0.9987999937711957</v>
+        <v>0.9988295373642557</v>
       </c>
       <c r="K13">
-        <v>0.9987999937711957</v>
+        <v>0.9988295373642557</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -840,34 +840,34 @@
         <v>375</v>
       </c>
       <c r="B14">
-        <v>0.9987640945273146</v>
+        <v>0.9984442976486717</v>
       </c>
       <c r="C14">
-        <v>0.9986675908013671</v>
+        <v>0.9986458077005917</v>
       </c>
       <c r="D14">
-        <v>0.9987648663792152</v>
+        <v>0.9986657443512555</v>
       </c>
       <c r="E14">
-        <v>0.998647970376189</v>
+        <v>0.9987222817995919</v>
       </c>
       <c r="F14">
-        <v>0.9987647373194586</v>
+        <v>0.998739693005412</v>
       </c>
       <c r="G14">
-        <v>0.9988203082782018</v>
+        <v>0.9988320827321372</v>
       </c>
       <c r="H14">
-        <v>0.9988203082782018</v>
+        <v>0.998856162093341</v>
       </c>
       <c r="I14">
-        <v>0.9988203082782018</v>
+        <v>0.9988420126856432</v>
       </c>
       <c r="J14">
-        <v>0.9988203082782018</v>
+        <v>0.9988420126856432</v>
       </c>
       <c r="K14">
-        <v>0.9988203082782018</v>
+        <v>0.9988420126856432</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -875,34 +875,34 @@
         <v>400</v>
       </c>
       <c r="B15">
-        <v>0.9987666545766982</v>
+        <v>0.9984784131782491</v>
       </c>
       <c r="C15">
-        <v>0.9986575197055354</v>
+        <v>0.9986491174738304</v>
       </c>
       <c r="D15">
-        <v>0.9987826601075105</v>
+        <v>0.9986757370223744</v>
       </c>
       <c r="E15">
-        <v>0.9986607361728937</v>
+        <v>0.998718139791732</v>
       </c>
       <c r="F15">
-        <v>0.9987799742120096</v>
+        <v>0.9987421910044108</v>
       </c>
       <c r="G15">
-        <v>0.9988305140255228</v>
+        <v>0.9988387304271393</v>
       </c>
       <c r="H15">
-        <v>0.9988305140255228</v>
+        <v>0.9988536461828972</v>
       </c>
       <c r="I15">
-        <v>0.9988305140255228</v>
+        <v>0.9988420095029171</v>
       </c>
       <c r="J15">
-        <v>0.9988305140255228</v>
+        <v>0.9988420095029171</v>
       </c>
       <c r="K15">
-        <v>0.9988305140255228</v>
+        <v>0.9988420095029171</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -910,34 +910,34 @@
         <v>425</v>
       </c>
       <c r="B16">
-        <v>0.99877171297359</v>
+        <v>0.9985066991938508</v>
       </c>
       <c r="C16">
-        <v>0.9985964471247601</v>
+        <v>0.9986324508881097</v>
       </c>
       <c r="D16">
-        <v>0.9987674007837567</v>
+        <v>0.9986665490986978</v>
       </c>
       <c r="E16">
-        <v>0.9986327214646268</v>
+        <v>0.9987206230757899</v>
       </c>
       <c r="F16">
-        <v>0.9987774518264791</v>
+        <v>0.9987380157088193</v>
       </c>
       <c r="G16">
-        <v>0.9988355692087753</v>
+        <v>0.9988204051038387</v>
       </c>
       <c r="H16">
-        <v>0.9988355692087753</v>
+        <v>0.9988403098307964</v>
       </c>
       <c r="I16">
-        <v>0.9988355692087753</v>
+        <v>0.9988378444581836</v>
       </c>
       <c r="J16">
-        <v>0.9988355692087753</v>
+        <v>0.9988378444581836</v>
       </c>
       <c r="K16">
-        <v>0.9988355692087753</v>
+        <v>0.9988378444581836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>